<commit_message>
Fill NaN with string 'Missing'
</commit_message>
<xml_diff>
--- a/FIO_Field_Descriptions.xlsx
+++ b/FIO_Field_Descriptions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>FIO Column Descriptions</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>0 = vehicle, 1 = passenger, -1 = NaN</t>
+  </si>
+  <si>
+    <t>0 = no, 1  = yes, -1 = unknown/NaN</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -718,7 +721,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -772,6 +775,9 @@
       <c r="B13" t="s">
         <v>75</v>
       </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -985,7 +991,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">

</xml_diff>